<commit_message>
Removed whitespaces from cells
</commit_message>
<xml_diff>
--- a/DATA EXCEL/CorrectCredentials.xlsx
+++ b/DATA EXCEL/CorrectCredentials.xlsx
@@ -28,16 +28,16 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_user </t>
+    <t xml:space="preserve">standard_user</t>
   </si>
   <si>
-    <t xml:space="preserve">secret_sauce </t>
+    <t xml:space="preserve">secret_sauce</t>
   </si>
   <si>
-    <t xml:space="preserve">problem_user </t>
+    <t xml:space="preserve">problem_user</t>
   </si>
   <si>
-    <t xml:space="preserve">performance_glitch_user </t>
+    <t xml:space="preserve">performance_glitch_user</t>
   </si>
 </sst>
 </file>
@@ -140,12 +140,12 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>